<commit_message>
Everything finshed but last graph
</commit_message>
<xml_diff>
--- a/lab 4/Lab4 2018 template(rev 0).xlsx
+++ b/lab 4/Lab4 2018 template(rev 0).xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
   <workbookPr date1904="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyStuff\MyDocs\Programming Projects\dataplotting\lab 4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ikmuj\OneDrive\Documents\Programming\dataplotting\lab 4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0BA52F7B-28A0-4DF0-B928-8A0D755F2485}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3929A64C-31E6-49FE-B376-67A5784AE523}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="32760" yWindow="32760" windowWidth="21600" windowHeight="11025" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="111">
   <si>
     <t>ECE2100 Lab #4 - Operation Amplifier Circuits</t>
   </si>
@@ -279,31 +279,803 @@
     <t>From Open Loop Voltage Gain vs. Frequency Plot</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Gain = </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
+    <t>Closed Loop Bandwidth Spec</t>
+  </si>
+  <si>
+    <t>(place screen shot here for break frequency illustration)</t>
+  </si>
+  <si>
+    <t>Comment on Closed Loop Gain-BW Product</t>
+  </si>
+  <si>
+    <t>(Screen Shot #2)</t>
+  </si>
+  <si>
+    <t>Differentiating Amplifier Circuit</t>
+  </si>
+  <si>
+    <t>Differentiating Amplifier Waveforms</t>
+  </si>
+  <si>
+    <t>(place waveforms here for triangular wave response)</t>
+  </si>
+  <si>
+    <t>(place waveforms here for sine wave response)</t>
+  </si>
+  <si>
+    <t>(Screen Shot #3)</t>
+  </si>
+  <si>
+    <t>(Screen Shot #4)</t>
+  </si>
+  <si>
+    <r>
+      <t>Comments on Differentiating Amplifier:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">    Page 4 of 4                         Fall 2018</t>
+  </si>
+  <si>
+    <t>Comments on Differentiating Amp Continued:</t>
+  </si>
+  <si>
+    <t>Output Voltage Amplitude - Triangular Wave Excitation</t>
+  </si>
+  <si>
+    <t>(place measured versus predicted output voltage peak-to-peak</t>
+  </si>
+  <si>
+    <t>vs.triangular wave frequency. Use discrete points for measured</t>
+  </si>
+  <si>
+    <t>data and a smooth line for prediction.)</t>
+  </si>
+  <si>
+    <t>(Plot #4)</t>
+  </si>
+  <si>
+    <t>SMU1: Voltage Sweep: -10 to +10mV, 101 steps</t>
+  </si>
+  <si>
+    <t>SMU1: Voltage Sweep: -100 to +100mV, 101 steps</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SMU2:  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Voltage Meter: 10V Compliance</t>
+    </r>
+  </si>
+  <si>
+    <t>SMU2: Voltage Meter: 10V Compliance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  -0.05607657 to +0.03989327</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">98.09 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Symbol"/>
+      </rPr>
+      <t>W</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">  -0.01806778</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve"> to +0.02188172</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Voltage Gain </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>= 20log|v</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>out</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>/v</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>in</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>| = 20log|-71.108|= 37.038 dBs</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Scope:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Helv"/>
+      </rPr>
+      <t xml:space="preserve"> DC coupling &amp; CH1 triggering (external not working)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Func.Generator:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
         <color indexed="10"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>_____</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve"> dB = </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
+        <rFont val="Helv"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Helv"/>
+      </rPr>
+      <t>50mV P-t-P, Sine Wave, 100 Hz</t>
+    </r>
+  </si>
+  <si>
+    <t>Inverting Amplifoerat Break Frequency  (11.31 kHz)</t>
+  </si>
+  <si>
+    <r>
+      <t>Strangly, the left graph shows that there was a different V</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">CC- </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>on the UA741CP Op Amp than was on LF353. This is strange because we connected the same DC power supply to both Op Amps without changing any settings. The left  graph shows that linear response of the UA741CP Op Amp happened at a lower input voltage than that of the LF353. On the right graph, the measured input current was fluctuating around 0 for the LF353, so I wasn't able to get an accurate graph.</t>
+    </r>
+  </si>
+  <si>
+    <t>Date of Lab: 9/1/2018</t>
+  </si>
+  <si>
+    <r>
+      <t>Func.Generator:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
         <color indexed="10"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>_____</t>
+        <rFont val="Helv"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Helv"/>
+      </rPr>
+      <t>1V P-t-P, Triangle Wave, 200Hz</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Scope:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="10"/>
+        <rFont val="Helv"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Helv"/>
+      </rPr>
+      <t>DC Coupling, CH2 Resolution</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Func.Generator:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="10"/>
+        <rFont val="Helv"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Helv"/>
+      </rPr>
+      <t>1V P-t-P, Sine Wave, 200 Hz</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>I</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>IB</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve"> = 30 nA,    V</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>IO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve"> = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>1.2373</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve"> mV,    r</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>I</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve"> &gt; 0.04124 M</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Symbol"/>
+      </rPr>
+      <t>W</t>
+    </r>
+  </si>
+  <si>
+    <t>Inverting Amplifier:  R1 = .98721 W,    R2= 97.15 kW,    RL= 98.09 W    +/-Vcc=6.01, - 6.01V</t>
+  </si>
+  <si>
+    <r>
+      <t>Op Amp # UA741CP: (Gain)(BW) = N/A kHz, I</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>IB</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> = 20 nA, V</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>IO</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t> = 1 mV, r</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>in</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t> = 2 M</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
+      <t>W</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>, r</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>O</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> = 75 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
+      <t>W</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>, CMRR = 90 dB</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Op Amp # LF353: (Gain)(BW) = 4 MHz, I</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>IB</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t> = 50 pA, V</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>IO</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t> = 5 mV, r</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>in</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t> = 10</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>12</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
+      <t>W</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>, r</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>O</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve"> = N/A </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
+      <t>W</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>, CMRR = 100 dB</t>
+    </r>
+  </si>
+  <si>
+    <t>For the Closed Loop, the linear response had a much larger range than that of the open loop. Whereas the open loop saw a sudden spike in voltage between saturation voltages, the closed loop saw a very gradual change between staturation voltages.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">  -VM  = -10mV - Vcc</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve"> = -6.02 V</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">  +VM = 10mV + Vcc = +6.02 V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  -VM  = -10mV - Vcc = -6.02 V</t>
+  </si>
+  <si>
+    <r>
+      <t>I</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>IB</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve"> ~  9 pA,    V</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>IO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve"> = 3.035 mV,    r</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>I</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve"> &gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Symbol"/>
+      </rPr>
+      <t>W</t>
+    </r>
+  </si>
+  <si>
+    <t>Adding the output resistance reduced the range of the linear response in the op amp by appx. 0.56V. This is a significant change, compared to the original range of 0.9V, reducing the range by nearly half.</t>
+  </si>
+  <si>
+    <t>Change from 5.33V to 1.64V at positive stauration</t>
+  </si>
+  <si>
+    <t>Break Frequency = 11.31 kHz</t>
+  </si>
+  <si>
+    <r>
+      <t>Gain-BW =</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 47.86*11310</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> = 5.4129 (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>) Hz</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">|Vout/Vin| = 47.86 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>= 33.6 dB</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve">    Phase Shift =</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve"> -180 °</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">|Vout/Vin| = 52.52 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>= 34.406 dB</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve">    Phase Shift =122</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve"> °</t>
+    </r>
+  </si>
+  <si>
+    <t>Gain = 47.86 = 33.6 dB</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Gain = 40 dB = 100 </t>
     </r>
     <r>
       <rPr>
@@ -330,15 +1102,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Break Frequency = </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="10"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>____</t>
+      <t>Break Frequency = 100</t>
     </r>
     <r>
       <rPr>
@@ -350,7 +1114,7 @@
   </si>
   <si>
     <r>
-      <t>Gain-BW =</t>
+      <t xml:space="preserve">Gain-BW = 100*100 </t>
     </r>
     <r>
       <rPr>
@@ -358,29 +1122,14 @@
         <color indexed="10"/>
         <rFont val="Verdana"/>
       </rPr>
-      <t>[show calc.]</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="10"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>_____</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>(10</t>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>= 10000 (10</t>
     </r>
     <r>
       <rPr>
@@ -399,204 +1148,7 @@
     </r>
   </si>
   <si>
-    <t>Closed Loop Bandwidth Spec</t>
-  </si>
-  <si>
-    <r>
-      <t>Gain =</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="10"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>_____</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="10"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>_____</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve"> dB</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Break Frequency =</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="10"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>_____</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve"> kHz</t>
-    </r>
-  </si>
-  <si>
-    <t>(place screen shot here for break frequency illustration)</t>
-  </si>
-  <si>
-    <r>
-      <t>Gain-BW =</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color indexed="10"/>
-        <rFont val="Verdana"/>
-      </rPr>
-      <t xml:space="preserve"> [show calc.]</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve"> =</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="10"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>______</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>(10</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>5</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>) Hz</t>
-    </r>
-  </si>
-  <si>
-    <t>Comment on Closed Loop Gain-BW Product</t>
-  </si>
-  <si>
-    <t>(Screen Shot #2)</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">|Vout/Vin| = </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="10"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>_____</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="10"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>_____</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve"> dB</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve">    Phase Shift =</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve"> -</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="10"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>_____</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve"> °</t>
-    </r>
-  </si>
-  <si>
-    <t>Differentiating Amplifier Circuit</t>
-  </si>
-  <si>
-    <t>Differentiating Amplifier Waveforms</t>
-  </si>
-  <si>
-    <t>(place waveforms here for triangular wave response)</t>
-  </si>
-  <si>
-    <t>(place waveforms here for sine wave response)</t>
-  </si>
-  <si>
-    <t>(Screen Shot #3)</t>
-  </si>
-  <si>
-    <t>(Screen Shot #4)</t>
+    <t>Truthfully, I wasn't entirly sure on what to do for this part. I caluculated the Av at 1 Hz over sqrt 2, read the frequency, and multiplied the two numbers together to try and get the Gain, but the numbers were not as expected.</t>
   </si>
   <si>
     <r>
@@ -631,7 +1183,14 @@
         <color indexed="10"/>
         <rFont val="Helv"/>
       </rPr>
-      <t xml:space="preserve"> [formula]</t>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Helv"/>
+      </rPr>
+      <t>200 * | t%0.01-0.005 | - 0.5</t>
     </r>
   </si>
   <si>
@@ -667,704 +1226,46 @@
         <color indexed="10"/>
         <rFont val="Helv"/>
       </rPr>
-      <t xml:space="preserve"> [formula]</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Comments on Differentiating Amplifier:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
       <t xml:space="preserve"> </t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">    Page 4 of 4                         Fall 2018</t>
-  </si>
-  <si>
-    <t>Comments on Differentiating Amp Continued:</t>
-  </si>
-  <si>
-    <t>Output Voltage Amplitude - Triangular Wave Excitation</t>
-  </si>
-  <si>
-    <t>(place measured versus predicted output voltage peak-to-peak</t>
-  </si>
-  <si>
-    <t>vs.triangular wave frequency. Use discrete points for measured</t>
-  </si>
-  <si>
-    <t>data and a smooth line for prediction.)</t>
-  </si>
-  <si>
-    <t>(Plot #4)</t>
-  </si>
-  <si>
-    <t>SMU1: Voltage Sweep: -10 to +10mV, 101 steps</t>
-  </si>
-  <si>
-    <t>SMU1: Voltage Sweep: -100 to +100mV, 101 steps</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">SMU2:  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> Voltage Meter: 10V Compliance</t>
-    </r>
-  </si>
-  <si>
-    <t>SMU2: Voltage Meter: 10V Compliance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  -0.05607657 to +0.03989327</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">98.09 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Symbol"/>
-      </rPr>
-      <t>W</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">  -0.01806778</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve"> to +0.02188172</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Voltage Gain </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>= 20log|v</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>out</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>/v</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>in</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>| = 20log|-71.108|= 37.038 dBs</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Scope:</t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
         <rFont val="Helv"/>
       </rPr>
-      <t xml:space="preserve"> DC coupling &amp; CH1 triggering (external not working)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Func.Generator:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="10"/>
-        <rFont val="Helv"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
+      <t>sin(200pi*t- 90</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
         <sz val="10"/>
         <rFont val="Helv"/>
       </rPr>
-      <t>50mV P-t-P, Sine Wave, 100 Hz</t>
-    </r>
-  </si>
-  <si>
-    <t>Inverting Amplifoerat Break Frequency  (11.31 kHz)</t>
-  </si>
-  <si>
-    <r>
-      <t>Strangly, the left graph shows that there was a different V</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">CC- </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>on the UA741CP Op Amp than was on LF353. This is strange because we connected the same DC power supply to both Op Amps without changing any settings. The left  graph shows that linear response of the UA741CP Op Amp happened at a lower input voltage than that of the LF353. On the right graph, the measured input current was fluctuating around 0 for the LF353, so I wasn't able to get an accurate graph.</t>
-    </r>
-  </si>
-  <si>
-    <t>Date of Lab: 9/1/2018</t>
-  </si>
-  <si>
-    <r>
-      <t>Func.Generator:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="10"/>
-        <rFont val="Helv"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
+      <t>o</t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
         <rFont val="Helv"/>
       </rPr>
-      <t>1V P-t-P, Triangle Wave, 200Hz</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Scope:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="10"/>
-        <rFont val="Helv"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Helv"/>
-      </rPr>
-      <t>DC Coupling, CH2 Resolution</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Func.Generator:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="10"/>
-        <rFont val="Helv"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Helv"/>
-      </rPr>
-      <t>1V P-t-P, Sine Wave, 200 Hz</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>I</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>IB</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve"> = 30 nA,    V</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>IO</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve"> = </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>1.2373</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve"> mV,    r</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>I</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve"> &gt; 0.04124 M</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Symbol"/>
-      </rPr>
-      <t>W</t>
-    </r>
-  </si>
-  <si>
-    <t>Inverting Amplifier:  R1 = .98721 W,    R2= 97.15 kW,    RL= 98.09 W    +/-Vcc=6.01, - 6.01V</t>
-  </si>
-  <si>
-    <r>
-      <t>Op Amp # UA741CP: (Gain)(BW) = N/A kHz, I</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>IB</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> = 20 nA, V</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>IO</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t> = 1 mV, r</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>in</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t> = 2 M</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="Symbol"/>
-        <family val="1"/>
-        <charset val="2"/>
-      </rPr>
-      <t>W</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>, r</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>O</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> = 75 </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="Symbol"/>
-        <family val="1"/>
-        <charset val="2"/>
-      </rPr>
-      <t>W</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>, CMRR = 90 dB</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Op Amp # LF353: (Gain)(BW) = 4 MHz, I</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>IB</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t> = 50 pA, V</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>IO</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t> = 5 mV, r</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>in</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t> = 10</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="superscript"/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>12</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="Symbol"/>
-        <family val="1"/>
-        <charset val="2"/>
-      </rPr>
-      <t>W</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>, r</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>O</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve"> = N/A </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="Symbol"/>
-        <family val="1"/>
-        <charset val="2"/>
-      </rPr>
-      <t>W</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>, CMRR = 100 dB</t>
-    </r>
-  </si>
-  <si>
-    <t>For the Closed Loop, the linear response had a much larger range than that of the open loop. Whereas the open loop saw a sudden spike in voltage between saturation voltages, the closed loop saw a very gradual change between staturation voltages.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">  -VM  = -10mV - Vcc</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve"> = -6.02 V</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">  +VM = 10mV + Vcc = +6.02 V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  -VM  = -10mV - Vcc = -6.02 V</t>
-  </si>
-  <si>
-    <r>
-      <t>I</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>IB</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve"> ~  9 pA,    V</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>IO</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve"> = 3.035 mV,    r</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>I</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve"> &gt; </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Symbol"/>
-      </rPr>
-      <t>W</t>
-    </r>
-  </si>
-  <si>
-    <t>Adding the output resistance reduced the range of the linear response in the op amp by appx. 0.56V. This is a significant change, compared to the original range of 0.9V, reducing the range by nearly half.</t>
-  </si>
-  <si>
-    <t>Change from 5.33V to 1.64V at positive stauration</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">|Vout/Vin| = 2.68/0.028 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>= 47.86 dB</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve">    Phase Shift =</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve"> -180 °</t>
-    </r>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>There is a mini underdamped response from the capacitor at each change peak on the triangle wave, because each peak acts as if it was a stepping edge for dv/dt.</t>
+  </si>
+  <si>
+    <t>However, on the sinusoidal response, ther e is no clear evidence of an underdamped response on the graph, even though there is a constantly changing dv/dt.</t>
+  </si>
+  <si>
+    <t>No measured data was found in my lab materials.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -1474,6 +1375,16 @@
       <name val="Verdana"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="10"/>
+      <name val="Helv"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -2000,7 +1911,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="176">
+  <cellXfs count="182">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -2145,9 +2056,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2168,9 +2076,6 @@
       <alignment horizontal="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2194,6 +2099,105 @@
       <alignment horizontal="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2224,9 +2228,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2257,66 +2258,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -2326,12 +2267,6 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" shrinkToFit="1"/>
     </xf>
@@ -2350,49 +2285,43 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3430,7 +3359,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -3474,7 +3403,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -3498,8 +3427,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z282"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="A140" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D154" sqref="D154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3527,8 +3456,8 @@
       <c r="B2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="100" t="s">
-        <v>91</v>
+      <c r="C2" s="98" t="s">
+        <v>82</v>
       </c>
       <c r="D2"/>
     </row>
@@ -3536,7 +3465,7 @@
       <c r="A3" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="90" t="s">
+      <c r="B3" s="89" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="17" t="s">
@@ -3548,48 +3477,48 @@
       <c r="A4" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="109"/>
-      <c r="C4" s="110"/>
+      <c r="B4" s="140"/>
+      <c r="C4" s="141"/>
       <c r="D4"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="111"/>
-      <c r="C5" s="112"/>
+      <c r="B5" s="142"/>
+      <c r="C5" s="143"/>
       <c r="D5"/>
     </row>
     <row r="6" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="113"/>
-      <c r="C6" s="114"/>
+      <c r="B6" s="144"/>
+      <c r="C6" s="145"/>
       <c r="D6"/>
     </row>
     <row r="7" spans="1:4" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="115" t="s">
+      <c r="A7" s="146" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="116"/>
+      <c r="B7" s="147"/>
       <c r="C7" s="10"/>
       <c r="D7"/>
     </row>
     <row r="8" spans="1:4" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="162" t="s">
-        <v>97</v>
-      </c>
-      <c r="B8" s="163"/>
-      <c r="C8" s="164"/>
+      <c r="A8" s="111" t="s">
+        <v>88</v>
+      </c>
+      <c r="B8" s="112"/>
+      <c r="C8" s="113"/>
       <c r="D8"/>
     </row>
     <row r="9" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="165" t="s">
-        <v>98</v>
-      </c>
-      <c r="B9" s="166"/>
-      <c r="C9" s="167"/>
+      <c r="A9" s="114" t="s">
+        <v>89</v>
+      </c>
+      <c r="B9" s="115"/>
+      <c r="C9" s="116"/>
       <c r="D9"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -3601,19 +3530,19 @@
       <c r="D10"/>
     </row>
     <row r="11" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="168" t="s">
-        <v>96</v>
-      </c>
-      <c r="B11" s="169"/>
-      <c r="C11" s="170"/>
+      <c r="A11" s="117" t="s">
+        <v>87</v>
+      </c>
+      <c r="B11" s="118"/>
+      <c r="C11" s="119"/>
       <c r="D11"/>
     </row>
     <row r="12" spans="1:4" s="8" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="171" t="s">
+      <c r="A12" s="120" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="172"/>
-      <c r="C12" s="173"/>
+      <c r="B12" s="121"/>
+      <c r="C12" s="122"/>
       <c r="D12"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -3627,38 +3556,38 @@
       <c r="D13"/>
     </row>
     <row r="14" spans="1:4" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="153" t="s">
-        <v>79</v>
-      </c>
-      <c r="B14" s="154"/>
-      <c r="C14" s="91" t="s">
+      <c r="A14" s="107" t="s">
+        <v>70</v>
+      </c>
+      <c r="B14" s="108"/>
+      <c r="C14" s="90" t="s">
         <v>15</v>
       </c>
       <c r="D14"/>
     </row>
     <row r="15" spans="1:4" ht="18.75" x14ac:dyDescent="0.35">
-      <c r="A15" s="148" t="s">
-        <v>82</v>
-      </c>
-      <c r="B15" s="149"/>
-      <c r="C15" s="103" t="s">
-        <v>95</v>
+      <c r="A15" s="109" t="s">
+        <v>73</v>
+      </c>
+      <c r="B15" s="139"/>
+      <c r="C15" s="101" t="s">
+        <v>86</v>
       </c>
       <c r="D15"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="25"/>
       <c r="B16" s="39"/>
-      <c r="C16" s="104" t="s">
-        <v>100</v>
+      <c r="C16" s="102" t="s">
+        <v>91</v>
       </c>
       <c r="D16"/>
     </row>
     <row r="17" spans="1:26" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="25"/>
       <c r="B17" s="39"/>
-      <c r="C17" s="106" t="s">
-        <v>101</v>
+      <c r="C17" s="104" t="s">
+        <v>92</v>
       </c>
       <c r="D17"/>
     </row>
@@ -3673,24 +3602,24 @@
     <row r="19" spans="1:26" ht="18.75" x14ac:dyDescent="0.35">
       <c r="A19" s="25"/>
       <c r="B19" s="39"/>
-      <c r="C19" s="104" t="s">
-        <v>103</v>
+      <c r="C19" s="102" t="s">
+        <v>94</v>
       </c>
       <c r="D19"/>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20" s="25"/>
       <c r="B20" s="39"/>
-      <c r="C20" s="104" t="s">
-        <v>102</v>
+      <c r="C20" s="102" t="s">
+        <v>93</v>
       </c>
       <c r="D20"/>
     </row>
     <row r="21" spans="1:26" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="25"/>
       <c r="B21" s="39"/>
-      <c r="C21" s="106" t="s">
-        <v>101</v>
+      <c r="C21" s="104" t="s">
+        <v>92</v>
       </c>
       <c r="D21"/>
     </row>
@@ -3883,47 +3812,47 @@
       <c r="C38" s="24"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="123" t="s">
-        <v>90</v>
-      </c>
-      <c r="B39" s="124"/>
-      <c r="C39" s="125"/>
+      <c r="A39" s="153" t="s">
+        <v>81</v>
+      </c>
+      <c r="B39" s="154"/>
+      <c r="C39" s="155"/>
       <c r="D39"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="126"/>
-      <c r="B40" s="124"/>
-      <c r="C40" s="125"/>
+      <c r="A40" s="156"/>
+      <c r="B40" s="154"/>
+      <c r="C40" s="155"/>
       <c r="D40"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="126"/>
-      <c r="B41" s="124"/>
-      <c r="C41" s="125"/>
+      <c r="A41" s="156"/>
+      <c r="B41" s="154"/>
+      <c r="C41" s="155"/>
       <c r="D41"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="126"/>
-      <c r="B42" s="124"/>
-      <c r="C42" s="125"/>
+      <c r="A42" s="156"/>
+      <c r="B42" s="154"/>
+      <c r="C42" s="155"/>
       <c r="D42"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="126"/>
-      <c r="B43" s="124"/>
-      <c r="C43" s="125"/>
+      <c r="A43" s="156"/>
+      <c r="B43" s="154"/>
+      <c r="C43" s="155"/>
       <c r="D43"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="126"/>
-      <c r="B44" s="124"/>
-      <c r="C44" s="125"/>
+      <c r="A44" s="156"/>
+      <c r="B44" s="154"/>
+      <c r="C44" s="155"/>
       <c r="D44"/>
     </row>
     <row r="45" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="127"/>
-      <c r="B45" s="128"/>
-      <c r="C45" s="129"/>
+      <c r="A45" s="157"/>
+      <c r="B45" s="158"/>
+      <c r="C45" s="159"/>
       <c r="D45"/>
     </row>
     <row r="46" spans="1:4" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3944,28 +3873,28 @@
       <c r="C47" s="34"/>
     </row>
     <row r="48" spans="1:4" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="174" t="s">
+      <c r="A48" s="123" t="s">
         <v>32</v>
       </c>
-      <c r="B48" s="175"/>
-      <c r="C48" s="96" t="s">
+      <c r="B48" s="124"/>
+      <c r="C48" s="95" t="s">
         <v>33</v>
       </c>
       <c r="D48"/>
     </row>
     <row r="49" spans="1:4" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="153" t="s">
-        <v>80</v>
-      </c>
-      <c r="B49" s="154"/>
+      <c r="A49" s="107" t="s">
+        <v>71</v>
+      </c>
+      <c r="B49" s="108"/>
       <c r="C49" s="27"/>
       <c r="D49"/>
     </row>
     <row r="50" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="148" t="s">
-        <v>81</v>
-      </c>
-      <c r="B50" s="161"/>
+      <c r="A50" s="109" t="s">
+        <v>72</v>
+      </c>
+      <c r="B50" s="110"/>
       <c r="C50" s="28"/>
     </row>
     <row r="51" spans="1:4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -4039,31 +3968,31 @@
       <c r="C62" s="28"/>
     </row>
     <row r="63" spans="1:4" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="105" t="s">
+      <c r="A63" s="103" t="s">
         <v>39</v>
       </c>
       <c r="B63" s="52" t="s">
         <v>40</v>
       </c>
-      <c r="C63" s="108" t="s">
-        <v>105</v>
+      <c r="C63" s="106" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="64" spans="1:4" customFormat="1" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A64" s="51" t="s">
         <v>41</v>
       </c>
-      <c r="B64" s="92" t="s">
-        <v>83</v>
+      <c r="B64" s="91" t="s">
+        <v>74</v>
       </c>
       <c r="C64" s="28"/>
     </row>
     <row r="65" spans="1:3" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="93" t="s">
-        <v>84</v>
-      </c>
-      <c r="B65" s="94" t="s">
-        <v>85</v>
+      <c r="A65" s="92" t="s">
+        <v>75</v>
+      </c>
+      <c r="B65" s="93" t="s">
+        <v>76</v>
       </c>
       <c r="C65" s="28"/>
     </row>
@@ -4080,8 +4009,8 @@
     <row r="68" spans="1:3" customFormat="1" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A68" s="72"/>
       <c r="B68" s="73"/>
-      <c r="C68" s="95" t="s">
-        <v>86</v>
+      <c r="C68" s="94" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="69" spans="1:3" customFormat="1" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
@@ -4092,21 +4021,21 @@
       <c r="C69" s="24"/>
     </row>
     <row r="70" spans="1:3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="150" t="s">
-        <v>104</v>
-      </c>
-      <c r="B70" s="142"/>
-      <c r="C70" s="133"/>
+      <c r="A70" s="160" t="s">
+        <v>95</v>
+      </c>
+      <c r="B70" s="133"/>
+      <c r="C70" s="127"/>
     </row>
     <row r="71" spans="1:3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="132"/>
-      <c r="B71" s="142"/>
-      <c r="C71" s="133"/>
+      <c r="A71" s="126"/>
+      <c r="B71" s="133"/>
+      <c r="C71" s="127"/>
     </row>
     <row r="72" spans="1:3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="132"/>
-      <c r="B72" s="142"/>
-      <c r="C72" s="133"/>
+      <c r="A72" s="126"/>
+      <c r="B72" s="133"/>
+      <c r="C72" s="127"/>
     </row>
     <row r="73" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
@@ -4116,53 +4045,53 @@
       <c r="C73" s="4"/>
     </row>
     <row r="74" spans="1:3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="150" t="s">
-        <v>99</v>
-      </c>
-      <c r="B74" s="142"/>
-      <c r="C74" s="133"/>
+      <c r="A74" s="160" t="s">
+        <v>90</v>
+      </c>
+      <c r="B74" s="133"/>
+      <c r="C74" s="127"/>
     </row>
     <row r="75" spans="1:3" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A75" s="132"/>
-      <c r="B75" s="142"/>
-      <c r="C75" s="133"/>
+      <c r="A75" s="126"/>
+      <c r="B75" s="133"/>
+      <c r="C75" s="127"/>
     </row>
     <row r="76" spans="1:3" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A76" s="132"/>
-      <c r="B76" s="142"/>
-      <c r="C76" s="133"/>
+      <c r="A76" s="126"/>
+      <c r="B76" s="133"/>
+      <c r="C76" s="127"/>
     </row>
     <row r="77" spans="1:3" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A77" s="132"/>
-      <c r="B77" s="142"/>
-      <c r="C77" s="133"/>
+      <c r="A77" s="126"/>
+      <c r="B77" s="133"/>
+      <c r="C77" s="127"/>
     </row>
     <row r="78" spans="1:3" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="134"/>
-      <c r="B78" s="143"/>
-      <c r="C78" s="135"/>
+      <c r="A78" s="128"/>
+      <c r="B78" s="134"/>
+      <c r="C78" s="129"/>
     </row>
     <row r="79" spans="1:3" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="159" t="s">
+      <c r="A79" s="167" t="s">
         <v>44</v>
       </c>
-      <c r="B79" s="160"/>
+      <c r="B79" s="168"/>
       <c r="C79" s="53" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="80" spans="1:3" customFormat="1" ht="16.5" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="153" t="s">
-        <v>88</v>
-      </c>
-      <c r="B80" s="154"/>
+      <c r="A80" s="107" t="s">
+        <v>79</v>
+      </c>
+      <c r="B80" s="108"/>
       <c r="C80" s="27"/>
     </row>
     <row r="81" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="151" t="s">
-        <v>87</v>
-      </c>
-      <c r="B81" s="152"/>
+      <c r="A81" s="161" t="s">
+        <v>78</v>
+      </c>
+      <c r="B81" s="162"/>
       <c r="C81" s="28"/>
     </row>
     <row r="82" spans="1:4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -4236,8 +4165,8 @@
     <row r="94" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" s="70"/>
       <c r="B94" s="71"/>
-      <c r="C94" s="107" t="s">
-        <v>106</v>
+      <c r="C94" s="105" t="s">
+        <v>99</v>
       </c>
       <c r="D94"/>
     </row>
@@ -4252,114 +4181,116 @@
       <c r="D95"/>
     </row>
     <row r="96" spans="1:4" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A96" s="157" t="s">
+      <c r="A96" s="165" t="s">
         <v>50</v>
       </c>
-      <c r="B96" s="158"/>
-      <c r="C96" s="98" t="s">
-        <v>89</v>
+      <c r="B96" s="166"/>
+      <c r="C96" s="96" t="s">
+        <v>80</v>
       </c>
       <c r="D96"/>
     </row>
     <row r="97" spans="1:4" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="155" t="s">
+      <c r="A97" s="163" t="s">
         <v>51</v>
       </c>
-      <c r="B97" s="156"/>
+      <c r="B97" s="164"/>
       <c r="C97" s="31"/>
       <c r="D97"/>
     </row>
     <row r="98" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A98" s="136" t="s">
-        <v>52</v>
-      </c>
-      <c r="B98" s="137"/>
+      <c r="A98" s="170" t="s">
+        <v>102</v>
+      </c>
+      <c r="B98" s="130"/>
       <c r="C98" s="4"/>
       <c r="D98"/>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" s="138" t="s">
-        <v>53</v>
-      </c>
-      <c r="B99" s="139"/>
+      <c r="A99" s="173" t="s">
+        <v>103</v>
+      </c>
+      <c r="B99" s="131"/>
       <c r="C99" s="4"/>
       <c r="D99"/>
     </row>
     <row r="100" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A100" s="140" t="s">
-        <v>54</v>
-      </c>
-      <c r="B100" s="141"/>
+      <c r="A100" s="172" t="s">
+        <v>104</v>
+      </c>
+      <c r="B100" s="132"/>
       <c r="C100" s="4"/>
       <c r="D100"/>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="75" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B101" s="74"/>
       <c r="C101" s="4"/>
       <c r="D101"/>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="136" t="s">
-        <v>56</v>
-      </c>
-      <c r="B102" s="137"/>
+      <c r="A102" s="170" t="s">
+        <v>101</v>
+      </c>
+      <c r="B102" s="130"/>
       <c r="C102" s="4"/>
       <c r="D102"/>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="138" t="s">
-        <v>57</v>
-      </c>
-      <c r="B103" s="139"/>
+      <c r="A103" s="173" t="s">
+        <v>97</v>
+      </c>
+      <c r="B103" s="131"/>
       <c r="C103" s="87" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D103" s="8"/>
     </row>
     <row r="104" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A104" s="119" t="s">
-        <v>59</v>
-      </c>
-      <c r="B104" s="120"/>
+      <c r="A104" s="169" t="s">
+        <v>98</v>
+      </c>
+      <c r="B104" s="150"/>
       <c r="C104" s="83" t="s">
         <v>47</v>
       </c>
       <c r="D104" s="8"/>
     </row>
     <row r="105" spans="1:4" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A105" s="121" t="s">
-        <v>60</v>
-      </c>
-      <c r="B105" s="122"/>
+      <c r="A105" s="151" t="s">
+        <v>54</v>
+      </c>
+      <c r="B105" s="152"/>
       <c r="C105" s="83" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D105"/>
     </row>
     <row r="106" spans="1:4" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="130"/>
-      <c r="B106" s="131"/>
+      <c r="A106" s="175" t="s">
+        <v>105</v>
+      </c>
+      <c r="B106" s="176"/>
       <c r="C106" s="4"/>
       <c r="D106"/>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="132"/>
-      <c r="B107" s="133"/>
+      <c r="A107" s="177"/>
+      <c r="B107" s="178"/>
       <c r="C107" s="4"/>
       <c r="D107"/>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="132"/>
-      <c r="B108" s="133"/>
+      <c r="A108" s="177"/>
+      <c r="B108" s="178"/>
       <c r="C108" s="4"/>
       <c r="D108"/>
     </row>
     <row r="109" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="134"/>
-      <c r="B109" s="135"/>
+      <c r="A109" s="179"/>
+      <c r="B109" s="180"/>
       <c r="C109" s="4"/>
       <c r="D109"/>
     </row>
@@ -4378,14 +4309,14 @@
     <row r="112" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A112" s="78"/>
       <c r="B112" s="73"/>
-      <c r="C112" s="97" t="s">
-        <v>62</v>
+      <c r="C112" s="171" t="s">
+        <v>100</v>
       </c>
       <c r="D112"/>
     </row>
     <row r="113" spans="1:4" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A113" s="81" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="B113" s="80"/>
       <c r="C113" s="79"/>
@@ -4442,28 +4373,28 @@
     <row r="122" spans="1:4" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A122" s="56"/>
       <c r="B122" s="57" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C122" s="58"/>
       <c r="D122"/>
     </row>
     <row r="123" spans="1:4" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="146" t="s">
-        <v>92</v>
-      </c>
-      <c r="B123" s="147"/>
-      <c r="C123" s="101" t="s">
-        <v>94</v>
+      <c r="A123" s="137" t="s">
+        <v>83</v>
+      </c>
+      <c r="B123" s="138"/>
+      <c r="C123" s="99" t="s">
+        <v>85</v>
       </c>
       <c r="D123"/>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A124" s="148" t="s">
-        <v>93</v>
-      </c>
-      <c r="B124" s="149"/>
-      <c r="C124" s="102" t="s">
-        <v>93</v>
+      <c r="A124" s="109" t="s">
+        <v>84</v>
+      </c>
+      <c r="B124" s="139"/>
+      <c r="C124" s="100" t="s">
+        <v>84</v>
       </c>
       <c r="D124"/>
     </row>
@@ -4499,21 +4430,21 @@
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" s="86" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="B130" s="4"/>
       <c r="C130" s="83" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="D130"/>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="85" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="B131" s="4"/>
       <c r="C131" s="83" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="D131"/>
     </row>
@@ -4554,33 +4485,35 @@
       <c r="D137"/>
     </row>
     <row r="138" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A138" s="117" t="s">
-        <v>69</v>
-      </c>
-      <c r="B138" s="118"/>
-      <c r="C138" s="88" t="s">
-        <v>70</v>
+      <c r="A138" s="148" t="s">
+        <v>106</v>
+      </c>
+      <c r="B138" s="149"/>
+      <c r="C138" s="181" t="s">
+        <v>107</v>
       </c>
       <c r="D138"/>
     </row>
     <row r="139" spans="1:4" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A139" s="7" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="B139" s="30"/>
       <c r="C139" s="31"/>
       <c r="D139"/>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A140" s="132"/>
-      <c r="B140" s="142"/>
-      <c r="C140" s="133"/>
+      <c r="A140" s="160" t="s">
+        <v>108</v>
+      </c>
+      <c r="B140" s="133"/>
+      <c r="C140" s="127"/>
       <c r="D140"/>
     </row>
     <row r="141" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A141" s="134"/>
-      <c r="B141" s="143"/>
-      <c r="C141" s="135"/>
+      <c r="A141" s="128"/>
+      <c r="B141" s="134"/>
+      <c r="C141" s="129"/>
       <c r="D141"/>
     </row>
     <row r="142" spans="1:4" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4589,77 +4522,79 @@
       </c>
       <c r="B142" s="21"/>
       <c r="C142" s="22" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="D142"/>
     </row>
     <row r="143" spans="1:4" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A143" s="144" t="s">
-        <v>73</v>
-      </c>
-      <c r="B143" s="145"/>
-      <c r="C143" s="99" t="s">
-        <v>74</v>
+      <c r="A143" s="135" t="s">
+        <v>64</v>
+      </c>
+      <c r="B143" s="136"/>
+      <c r="C143" s="97" t="s">
+        <v>65</v>
       </c>
       <c r="D143"/>
     </row>
     <row r="144" spans="1:4" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A144" s="130"/>
-      <c r="B144" s="131"/>
+      <c r="A144" s="174" t="s">
+        <v>109</v>
+      </c>
+      <c r="B144" s="125"/>
       <c r="C144" s="55"/>
       <c r="D144"/>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A145" s="132"/>
-      <c r="B145" s="133"/>
+      <c r="A145" s="126"/>
+      <c r="B145" s="127"/>
       <c r="C145" s="42"/>
       <c r="D145"/>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A146" s="132"/>
-      <c r="B146" s="133"/>
+      <c r="A146" s="126"/>
+      <c r="B146" s="127"/>
       <c r="C146" s="42"/>
       <c r="D146"/>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A147" s="132"/>
-      <c r="B147" s="133"/>
+      <c r="A147" s="126"/>
+      <c r="B147" s="127"/>
       <c r="C147" s="42"/>
       <c r="D147"/>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A148" s="132"/>
-      <c r="B148" s="133"/>
+      <c r="A148" s="126"/>
+      <c r="B148" s="127"/>
       <c r="C148" s="42"/>
       <c r="D148"/>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A149" s="132"/>
-      <c r="B149" s="133"/>
+      <c r="A149" s="126"/>
+      <c r="B149" s="127"/>
       <c r="C149" s="42"/>
       <c r="D149"/>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A150" s="132"/>
-      <c r="B150" s="133"/>
-      <c r="C150" s="89" t="s">
-        <v>75</v>
+      <c r="A150" s="126"/>
+      <c r="B150" s="127"/>
+      <c r="C150" s="88" t="s">
+        <v>66</v>
       </c>
       <c r="D150"/>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A151" s="132"/>
-      <c r="B151" s="133"/>
-      <c r="C151" s="89" t="s">
-        <v>76</v>
+      <c r="A151" s="126"/>
+      <c r="B151" s="127"/>
+      <c r="C151" s="88" t="s">
+        <v>67</v>
       </c>
       <c r="D151"/>
     </row>
     <row r="152" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A152" s="134"/>
-      <c r="B152" s="135"/>
-      <c r="C152" s="89" t="s">
-        <v>77</v>
+      <c r="A152" s="128"/>
+      <c r="B152" s="129"/>
+      <c r="C152" s="88" t="s">
+        <v>68</v>
       </c>
       <c r="D152"/>
     </row>
@@ -4667,7 +4602,7 @@
       <c r="A153" s="59"/>
       <c r="B153" s="60"/>
       <c r="C153" s="83" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="D153"/>
     </row>
@@ -4680,7 +4615,9 @@
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" s="59"/>
       <c r="B155" s="60"/>
-      <c r="C155" s="42"/>
+      <c r="C155" s="102" t="s">
+        <v>110</v>
+      </c>
       <c r="D155"/>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
@@ -5129,25 +5066,6 @@
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A144:B152"/>
-    <mergeCell ref="A98:B98"/>
-    <mergeCell ref="A99:B99"/>
-    <mergeCell ref="A100:B100"/>
-    <mergeCell ref="A102:B102"/>
-    <mergeCell ref="A103:B103"/>
-    <mergeCell ref="A140:C141"/>
-    <mergeCell ref="A143:B143"/>
-    <mergeCell ref="A106:B109"/>
-    <mergeCell ref="A123:B123"/>
-    <mergeCell ref="A124:B124"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B6:C6"/>
@@ -5164,6 +5082,25 @@
     <mergeCell ref="A96:B96"/>
     <mergeCell ref="A79:B79"/>
     <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A144:B152"/>
+    <mergeCell ref="A98:B98"/>
+    <mergeCell ref="A99:B99"/>
+    <mergeCell ref="A100:B100"/>
+    <mergeCell ref="A102:B102"/>
+    <mergeCell ref="A103:B103"/>
+    <mergeCell ref="A140:C141"/>
+    <mergeCell ref="A143:B143"/>
+    <mergeCell ref="A106:B109"/>
+    <mergeCell ref="A123:B123"/>
+    <mergeCell ref="A124:B124"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A48:B48"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.22222222222222221" right="0.18888888888888888" top="0.3888888888888889" bottom="2.2222222222222223E-2" header="0.5" footer="0.5"/>

</xml_diff>